<commit_message>
Roller Coaster & Water Rides
</commit_message>
<xml_diff>
--- a/rollercoaster-usa.xlsx
+++ b/rollercoaster-usa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="1720" windowWidth="25600" windowHeight="15120" tabRatio="500"/>
+    <workbookView xWindow="11200" yWindow="1280" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="99">
   <si>
     <t>State</t>
   </si>
@@ -280,6 +280,42 @@
   </si>
   <si>
     <t>Worlds of Fun</t>
+  </si>
+  <si>
+    <t>KS</t>
+  </si>
+  <si>
+    <t>Schlitterbanh Waterparks and Resort</t>
+  </si>
+  <si>
+    <t>Verrückt</t>
+  </si>
+  <si>
+    <t>1000+</t>
+  </si>
+  <si>
+    <t>WTR</t>
+  </si>
+  <si>
+    <t>WildeBeest</t>
+  </si>
+  <si>
+    <t>WI</t>
+  </si>
+  <si>
+    <t>Noah's Ark Waterpark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scorpion's Tail </t>
+  </si>
+  <si>
+    <t>Wisconsins Dells</t>
+  </si>
+  <si>
+    <t>San Dimas</t>
+  </si>
+  <si>
+    <t>Raging Waters</t>
   </si>
 </sst>
 </file>
@@ -685,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1343,50 +1379,110 @@
       <c r="I26" s="2"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
+      <c r="A27" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" s="2">
+        <v>168</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F27" s="2">
+        <v>65</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
+      <c r="A28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="2">
+        <v>64</v>
+      </c>
+      <c r="E28" s="2">
+        <v>1710</v>
+      </c>
+      <c r="F28" s="2">
+        <v>52.8</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
+      <c r="A29" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
+      <c r="E29" s="2">
+        <v>400</v>
+      </c>
+      <c r="F29" s="2">
+        <v>50</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
+      <c r="A30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" s="2">
+        <v>70</v>
+      </c>
       <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
+      <c r="F30" s="2">
+        <v>40</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
     </row>
@@ -1395,7 +1491,6 @@
     <sortCondition ref="B2:B30"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
roller coasters & water rides
</commit_message>
<xml_diff>
--- a/rollercoaster-usa.xlsx
+++ b/rollercoaster-usa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11200" yWindow="1280" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="100" yWindow="340" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -372,8 +372,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -387,9 +393,15 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -721,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -760,96 +772,104 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
+      <c r="A2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="3">
-        <v>5843</v>
-      </c>
-      <c r="E2" s="2"/>
+        <v>89</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="2">
+        <v>168</v>
+      </c>
       <c r="F2" s="2">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="2"/>
+        <v>31</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" s="2"/>
+        <v>92</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1710</v>
+      </c>
       <c r="E3" s="2">
-        <v>232</v>
+        <v>64</v>
       </c>
       <c r="F3" s="2">
-        <v>75</v>
+        <v>52.8</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>74</v>
+        <v>18</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2">
+        <v>456</v>
+      </c>
+      <c r="F4" s="2">
+        <v>128</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3">
-        <v>6595</v>
-      </c>
-      <c r="E4" s="2">
-        <v>310</v>
-      </c>
-      <c r="F4" s="2">
-        <v>93</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="3">
-        <v>5427</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+        <v>57</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2">
+        <v>420</v>
+      </c>
+      <c r="F5" s="2">
+        <v>120</v>
+      </c>
       <c r="G5" s="2" t="s">
         <v>14</v>
       </c>
@@ -857,218 +877,238 @@
         <v>15</v>
       </c>
       <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="F6" s="2">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" t="s">
-        <v>46</v>
+      <c r="A7" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="3">
-        <v>5400</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+        <v>95</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2">
+        <v>400</v>
+      </c>
+      <c r="F7" s="2">
+        <v>50</v>
+      </c>
       <c r="G7" s="2" t="s">
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D8" s="3">
-        <v>6072</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+        <v>6595</v>
+      </c>
+      <c r="E8" s="2">
+        <v>310</v>
+      </c>
+      <c r="F8" s="2">
+        <v>93</v>
+      </c>
       <c r="G8" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
+      <c r="A9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="3">
-        <v>5600</v>
-      </c>
-      <c r="E9" s="2"/>
+        <v>63</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2">
+        <v>305</v>
+      </c>
       <c r="F9" s="2">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="2" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2">
+        <v>245</v>
+      </c>
       <c r="F10" s="2">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2">
+        <v>235</v>
+      </c>
+      <c r="F11" s="2">
         <v>85</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2">
-        <v>75</v>
-      </c>
       <c r="G11" s="2" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
+      <c r="A12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="3">
-        <v>6442</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+        <v>73</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2">
+        <v>232</v>
+      </c>
+      <c r="F12" s="2">
+        <v>75</v>
+      </c>
       <c r="G12" s="2" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>75</v>
+        <v>8</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="E13" s="2">
+        <v>230</v>
+      </c>
       <c r="F13" s="2">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>76</v>
+        <v>11</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="D14" s="3">
+        <v>5394</v>
+      </c>
       <c r="E14" s="2">
-        <v>305</v>
+        <v>230</v>
       </c>
       <c r="F14" s="2">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>55</v>
@@ -1078,387 +1118,359 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="3">
+        <v>5843</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2">
+        <v>80</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
         <v>7</v>
       </c>
-      <c r="B15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="3">
-        <v>7359</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>8</v>
+      <c r="B16" t="s">
+        <v>12</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2">
-        <v>230</v>
-      </c>
-      <c r="F16" s="2">
-        <v>80</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="D16" s="3">
+        <v>5427</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
       <c r="G16" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="2" t="s">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="3">
+        <v>5400</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2">
-        <v>82</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>50</v>
+      <c r="B18" t="s">
+        <v>22</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="D18" s="3">
-        <v>5394</v>
-      </c>
-      <c r="E18" s="2">
-        <v>230</v>
-      </c>
-      <c r="F18" s="2">
-        <v>80</v>
-      </c>
+        <v>6072</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
       <c r="G18" s="2" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>50</v>
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2">
-        <v>456</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="D19" s="3">
+        <v>5600</v>
+      </c>
+      <c r="E19" s="2"/>
       <c r="F19" s="2">
-        <v>128</v>
+        <v>75</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="2" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="D20" s="2"/>
-      <c r="E20" s="2">
-        <v>415</v>
-      </c>
+      <c r="E20" s="2"/>
       <c r="F20" s="2">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="2" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="D21" s="2"/>
-      <c r="E21" s="2">
-        <v>235</v>
-      </c>
+      <c r="E21" s="2"/>
       <c r="F21" s="2">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>58</v>
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" t="s">
+        <v>19</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D22" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="D22" s="3">
+        <v>6442</v>
+      </c>
       <c r="E22" s="2"/>
-      <c r="F22" s="2">
-        <v>76</v>
-      </c>
+      <c r="F22" s="2"/>
       <c r="G22" s="2" t="s">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" t="s">
-        <v>43</v>
+      <c r="A23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="3">
-        <v>5400</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>40</v>
       </c>
       <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>66</v>
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2">
-        <v>245</v>
-      </c>
-      <c r="F24" s="2">
-        <v>85</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D24" s="3">
+        <v>7359</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
       <c r="G24" s="2" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="H24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2">
+        <v>82</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" s="3">
-        <v>5460</v>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" t="s">
-        <v>86</v>
+      <c r="A26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="3">
-        <v>5600</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2">
+        <v>76</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="3">
+        <v>5400</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2">
+        <v>77</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="3">
+        <v>5460</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="3">
+        <v>5600</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2">
         <v>75</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G29" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H29" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I26" s="2"/>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D27" s="2">
-        <v>168</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F27" s="2">
-        <v>65</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D28" s="2">
-        <v>64</v>
-      </c>
-      <c r="E28" s="2">
-        <v>1710</v>
-      </c>
-      <c r="F28" s="2">
-        <v>52.8</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2">
-        <v>400</v>
-      </c>
-      <c r="F29" s="2">
-        <v>50</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="2" t="s">
@@ -1470,10 +1482,9 @@
       <c r="C30" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D30" s="2">
+      <c r="E30" s="2">
         <v>70</v>
       </c>
-      <c r="E30" s="2"/>
       <c r="F30" s="2">
         <v>40</v>
       </c>
@@ -1488,9 +1499,10 @@
     </row>
   </sheetData>
   <sortState ref="A2:J30">
-    <sortCondition ref="B2:B30"/>
+    <sortCondition descending="1" ref="E2:E30"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>